<commit_message>
All Lab 2 Files
</commit_message>
<xml_diff>
--- a/Lab2/Lab2_report_table.xlsx
+++ b/Lab2/Lab2_report_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="280" uniqueCount="12">
   <si>
     <t>Type</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>Diseased State</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -119,7 +125,7 @@
         <v>70.826306913996632</v>
       </c>
       <c r="C2" s="0">
-        <v>61.696658097686381</v>
+        <v>185.21983161833489</v>
       </c>
     </row>
     <row r="3">
@@ -151,8 +157,8 @@
       <c r="B5" s="0">
         <v>0.075625000000000067</v>
       </c>
-      <c r="C5" s="0">
-        <v>0.16318181818181834</v>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -162,8 +168,8 @@
       <c r="B6" s="0">
         <v>0.11249999999999998</v>
       </c>
-      <c r="C6" s="0">
-        <v>0.32318181818181829</v>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -173,8 +179,8 @@
       <c r="B7" s="0">
         <v>0.30187499999999989</v>
       </c>
-      <c r="C7" s="0">
-        <v>0.48363636363636359</v>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8">

</xml_diff>